<commit_message>
Write player noo set in plusminus.xlsx
</commit_message>
<xml_diff>
--- a/basketBallRecorder/Xlsx/Plus Minus.xlsx
+++ b/basketBallRecorder/Xlsx/Plus Minus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27021"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -422,7 +422,7 @@
   <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -431,6 +431,7 @@
     <col min="11" max="11" width="8" customWidth="1"/>
     <col min="12" max="12" width="9.83203125" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">

</xml_diff>

<commit_message>
Finish plus minus upload in menu
</commit_message>
<xml_diff>
--- a/basketBallRecorder/Xlsx/Plus Minus.xlsx
+++ b/basketBallRecorder/Xlsx/Plus Minus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27021"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +109,24 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -127,21 +145,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="11" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -411,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -419,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -432,6 +501,7 @@
     <col min="12" max="12" width="9.83203125" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -477,20 +547,1801 @@
       <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2">
+        <f>SUM(S2:W2)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <f>SUMIF(A$2:A$5,$P2,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <f>SUMIF(B$2:B$5,$P2,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f>SUMIF(C$2:C$5,$P2,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f>SUMIF(D$2:D$5,$P2,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <f>SUMIF(E$2:E$5,$P2,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2">
+        <f>SUM(S3:W3)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <f>SUMIF(A$2:A$5,$P3,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f>SUMIF(B$2:B$5,$P3,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f>SUMIF(C$2:C$5,$P3,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f>SUMIF(D$2:D$5,$P3,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>SUMIF(E$2:E$5,$P3,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2">
+        <f>SUM(S4:W4)</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <f>SUMIF(A$2:A$5,$P4,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f>SUMIF(B$2:B$5,$P4,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <f>SUMIF(C$2:C$5,$P4,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <f>SUMIF(D$2:D$5,$P4,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f>SUMIF(E$2:E$5,$P4,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2">
+        <f>SUM(S5:W5)</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <f>SUMIF(A$2:A$5,$P5,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f>SUMIF(B$2:B$5,$P5,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <f>SUMIF(C$2:C$5,$P5,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <f>SUMIF(D$2:D$5,$P5,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f>SUMIF(E$2:E$5,$P5,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2">
+        <f>SUM(S6:W6)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <f>SUMIF(A$2:A$5,$P6,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f>SUMIF(B$2:B$5,$P6,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f>SUMIF(C$2:C$5,$P6,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f>SUMIF(D$2:D$5,$P6,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f>SUMIF(E$2:E$5,$P6,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2">
+        <f>SUM(S7:W7)</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <f>SUMIF(A$2:A$5,$P7,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <f>SUMIF(B$2:B$5,$P7,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <f>SUMIF(C$2:C$5,$P7,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <f>SUMIF(D$2:D$5,$P7,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <f>SUMIF(E$2:E$5,$P7,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2">
+        <f>SUM(S8:W8)</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <f>SUMIF(A$2:A$5,$P8,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <f>SUMIF(B$2:B$5,$P8,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <f>SUMIF(C$2:C$5,$P8,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <f>SUMIF(D$2:D$5,$P8,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <f>SUMIF(E$2:E$5,$P8,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2">
+        <f>SUM(S9:W9)</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <f>SUMIF(A$2:A$5,$P9,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f>SUMIF(B$2:B$5,$P9,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f>SUMIF(C$2:C$5,$P9,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f>SUMIF(D$2:D$5,$P9,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <f>SUMIF(E$2:E$5,$P9,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2">
+        <f>SUM(S10:W10)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <f>SUMIF(A$2:A$5,$P10,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f>SUMIF(B$2:B$5,$P10,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f>SUMIF(C$2:C$5,$P10,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <f>SUMIF(D$2:D$5,$P10,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <f>SUMIF(E$2:E$5,$P10,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2">
+        <f>SUM(S11:W11)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <f>SUMIF(A$2:A$5,$P11,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f>SUMIF(B$2:B$5,$P11,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <f>SUMIF(C$2:C$5,$P11,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <f>SUMIF(D$2:D$5,$P11,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <f>SUMIF(E$2:E$5,$P11,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2">
+        <f>SUM(S12:W12)</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="2">
+        <f>SUMIF(A$2:A$5,$P12,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f>SUMIF(B$2:B$5,$P12,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f>SUMIF(C$2:C$5,$P12,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f>SUMIF(D$2:D$5,$P12,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <f>SUMIF(E$2:E$5,$P12,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2">
+        <f>SUM(S13:W13)</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <f>SUMIF(A$2:A$5,$P13,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f>SUMIF(B$2:B$5,$P13,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f>SUMIF(C$2:C$5,$P13,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <f>SUMIF(D$2:D$5,$P13,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f>SUMIF(E$2:E$5,$P13,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2">
+        <f>SUM(S14:W14)</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <f>SUMIF(A$2:A$5,$P14,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f>SUMIF(B$2:B$5,$P14,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f>SUMIF(C$2:C$5,$P14,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f>SUMIF(D$2:D$5,$P14,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <f>SUMIF(E$2:E$5,$P14,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2">
+        <f>SUM(S15:W15)</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <f>SUMIF(A$2:A$5,$P15,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f>SUMIF(B$2:B$5,$P15,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f>SUMIF(C$2:C$5,$P15,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f>SUMIF(D$2:D$5,$P15,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f>SUMIF(E$2:E$5,$P15,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2">
+        <f>SUM(S16:W16)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="2">
+        <f>SUMIF(A$2:A$5,$P16,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f>SUMIF(B$2:B$5,$P16,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f>SUMIF(C$2:C$5,$P16,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f>SUMIF(D$2:D$5,$P16,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <f>SUMIF(E$2:E$5,$P16,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:23">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2">
+        <f>SUM(S17:W17)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="2">
+        <f>SUMIF(A$2:A$5,$P17,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f>SUMIF(B$2:B$5,$P17,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f>SUMIF(C$2:C$5,$P17,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <f>SUMIF(D$2:D$5,$P17,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <f>SUMIF(E$2:E$5,$P17,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:23">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2">
+        <f>SUM(S18:W18)</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <f>SUMIF(A$2:A$5,$P18,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <f>SUMIF(B$2:B$5,$P18,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f>SUMIF(C$2:C$5,$P18,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <f>SUMIF(D$2:D$5,$P18,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <f>SUMIF(E$2:E$5,$P18,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:23">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2">
+        <f>SUM(S19:W19)</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="2">
+        <f>SUMIF(A$2:A$5,$P19,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f>SUMIF(B$2:B$5,$P19,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <f>SUMIF(C$2:C$5,$P19,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <f>SUMIF(D$2:D$5,$P19,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <f>SUMIF(E$2:E$5,$P19,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:23">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2">
+        <f>SUM(S20:W20)</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="2">
+        <f>SUMIF(A$2:A$5,$P20,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <f>SUMIF(B$2:B$5,$P20,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <f>SUMIF(C$2:C$5,$P20,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f>SUMIF(D$2:D$5,$P20,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <f>SUMIF(E$2:E$5,$P20,$J$2:$J$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:23">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="3:23">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="3:23">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="3:23">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="3:23">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="3:23">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="3:23">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="3:23">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="3:23">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="3:23">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="3:23">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="3:23">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" spans="3:17">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="3:17">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+    </row>
+    <row r="35" spans="3:17">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+    </row>
+    <row r="36" spans="3:17">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+    </row>
+    <row r="37" spans="3:17">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+    </row>
+    <row r="38" spans="3:17">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" spans="3:17">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="3:17">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+    </row>
+    <row r="41" spans="3:17">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+    </row>
+    <row r="42" spans="3:17">
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+    </row>
+    <row r="43" spans="3:17">
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+    </row>
+    <row r="44" spans="3:17">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+    </row>
+    <row r="45" spans="3:17">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+    </row>
+    <row r="46" spans="3:17">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+    </row>
+    <row r="47" spans="3:17">
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+    </row>
+    <row r="48" spans="3:17">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+    </row>
+    <row r="49" spans="3:17">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="3:17">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+    </row>
+    <row r="51" spans="3:17">
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="3:17">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+    </row>
+    <row r="53" spans="3:17">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+    </row>
+    <row r="54" spans="3:17">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+    </row>
+    <row r="55" spans="3:17">
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="3:17">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+    </row>
+    <row r="57" spans="3:17">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+    </row>
+    <row r="58" spans="3:17">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+    </row>
+    <row r="59" spans="3:17">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+    </row>
+    <row r="60" spans="3:17">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+    </row>
+    <row r="61" spans="3:17">
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+    </row>
+    <row r="62" spans="3:17">
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+    </row>
+    <row r="63" spans="3:17">
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+    </row>
+    <row r="64" spans="3:17">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
+    </row>
+    <row r="65" spans="3:17">
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2"/>
+    </row>
+    <row r="66" spans="3:17">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2"/>
+    </row>
+    <row r="67" spans="3:17">
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2"/>
+    </row>
+    <row r="68" spans="3:17">
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+    </row>
+    <row r="69" spans="3:17">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+    </row>
+    <row r="70" spans="3:17">
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2"/>
+    </row>
+    <row r="71" spans="3:17">
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+    </row>
+    <row r="72" spans="3:17">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
+    </row>
+    <row r="73" spans="3:17">
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
+    </row>
+    <row r="74" spans="3:17">
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+    </row>
+    <row r="75" spans="3:17">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+    </row>
+    <row r="76" spans="3:17">
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+    </row>
+    <row r="77" spans="3:17">
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+    </row>
+    <row r="78" spans="3:17">
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2"/>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+    </row>
+    <row r="79" spans="3:17">
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+      <c r="O79" s="2"/>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="2"/>
+    </row>
+    <row r="80" spans="3:17">
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <ignoredErrors>
+    <ignoredError sqref="S2:W20" emptyCellReference="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
DEBUG: fix the wrong function in plus_minus.xlsx
</commit_message>
<xml_diff>
--- a/basketBallRecorder/Xlsx/Plus Minus.xlsx
+++ b/basketBallRecorder/Xlsx/Plus Minus.xlsx
@@ -480,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -571,27 +571,27 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2">
-        <f>SUM(S2:W2)</f>
+        <f t="shared" ref="Q2:Q20" si="0">SUM(S2:W2)</f>
         <v>0</v>
       </c>
       <c r="S2" s="2">
-        <f>SUMIF(A$2:A$5,$P2,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <f>SUMIF(B$2:B$5,$P2,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <f>SUMIF(C$2:C$5,$P2,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <f>SUMIF(D$2:D$5,$P2,$J$2:$J$5)</f>
+        <f>SUMIF(A:A,$P2,$J:$J )</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <f t="shared" ref="T2:V17" si="1">SUMIF(B:B,$P2,$J:$J )</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V2" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W2">
-        <f>SUMIF(E$2:E$5,$P2,$J$2:$J$5)</f>
+        <f t="shared" ref="W2:W20" si="2">SUMIF(E$2:E$5,$P2,$J$2:$J$5)</f>
         <v>0</v>
       </c>
     </row>
@@ -611,27 +611,27 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2">
-        <f>SUM(S3:W3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S3" s="2">
-        <f>SUMIF(A$2:A$5,$P3,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <f>SUMIF(B$2:B$5,$P3,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <f>SUMIF(C$2:C$5,$P3,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <f>SUMIF(D$2:D$5,$P3,$J$2:$J$5)</f>
+        <f t="shared" ref="S3:S20" si="3">SUMIF(A:A,$P3,$J:$J )</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W3">
-        <f>SUMIF(E$2:E$5,$P3,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -651,27 +651,27 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2">
-        <f>SUM(S4:W4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S4" s="2">
-        <f>SUMIF(A$2:A$5,$P4,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <f>SUMIF(B$2:B$5,$P4,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <f>SUMIF(C$2:C$5,$P4,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <f>SUMIF(D$2:D$5,$P4,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W4">
-        <f>SUMIF(E$2:E$5,$P4,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -691,27 +691,27 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2">
-        <f>SUM(S5:W5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S5" s="2">
-        <f>SUMIF(A$2:A$5,$P5,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <f>SUMIF(B$2:B$5,$P5,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <f>SUMIF(C$2:C$5,$P5,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <f>SUMIF(D$2:D$5,$P5,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W5">
-        <f>SUMIF(E$2:E$5,$P5,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -731,27 +731,27 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2">
-        <f>SUM(S6:W6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S6" s="2">
-        <f>SUMIF(A$2:A$5,$P6,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <f>SUMIF(B$2:B$5,$P6,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <f>SUMIF(C$2:C$5,$P6,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <f>SUMIF(D$2:D$5,$P6,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W6">
-        <f>SUMIF(E$2:E$5,$P6,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -771,27 +771,27 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2">
-        <f>SUM(S7:W7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S7" s="2">
-        <f>SUMIF(A$2:A$5,$P7,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <f>SUMIF(B$2:B$5,$P7,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <f>SUMIF(C$2:C$5,$P7,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <f>SUMIF(D$2:D$5,$P7,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W7">
-        <f>SUMIF(E$2:E$5,$P7,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -811,27 +811,27 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2">
-        <f>SUM(S8:W8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S8" s="2">
-        <f>SUMIF(A$2:A$5,$P8,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <f>SUMIF(B$2:B$5,$P8,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <f>SUMIF(C$2:C$5,$P8,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <f>SUMIF(D$2:D$5,$P8,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W8">
-        <f>SUMIF(E$2:E$5,$P8,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -851,27 +851,27 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2">
-        <f>SUM(S9:W9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S9" s="2">
-        <f>SUMIF(A$2:A$5,$P9,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <f>SUMIF(B$2:B$5,$P9,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <f>SUMIF(C$2:C$5,$P9,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <f>SUMIF(D$2:D$5,$P9,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W9">
-        <f>SUMIF(E$2:E$5,$P9,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -891,27 +891,27 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2">
-        <f>SUM(S10:W10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S10" s="2">
-        <f>SUMIF(A$2:A$5,$P10,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <f>SUMIF(B$2:B$5,$P10,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <f>SUMIF(C$2:C$5,$P10,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <f>SUMIF(D$2:D$5,$P10,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W10">
-        <f>SUMIF(E$2:E$5,$P10,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -931,27 +931,27 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2">
-        <f>SUM(S11:W11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S11" s="2">
-        <f>SUMIF(A$2:A$5,$P11,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <f>SUMIF(B$2:B$5,$P11,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <f>SUMIF(C$2:C$5,$P11,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <f>SUMIF(D$2:D$5,$P11,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W11">
-        <f>SUMIF(E$2:E$5,$P11,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -971,27 +971,27 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2">
-        <f>SUM(S12:W12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S12" s="2">
-        <f>SUMIF(A$2:A$5,$P12,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <f>SUMIF(B$2:B$5,$P12,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <f>SUMIF(C$2:C$5,$P12,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <f>SUMIF(D$2:D$5,$P12,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W12">
-        <f>SUMIF(E$2:E$5,$P12,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1011,27 +1011,27 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2">
-        <f>SUM(S13:W13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S13" s="2">
-        <f>SUMIF(A$2:A$5,$P13,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <f>SUMIF(B$2:B$5,$P13,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <f>SUMIF(C$2:C$5,$P13,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <f>SUMIF(D$2:D$5,$P13,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f>SUMIF(E$2:E$5,$P13,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1051,27 +1051,27 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2">
-        <f>SUM(S14:W14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S14" s="2">
-        <f>SUMIF(A$2:A$5,$P14,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <f>SUMIF(B$2:B$5,$P14,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <f>SUMIF(C$2:C$5,$P14,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <f>SUMIF(D$2:D$5,$P14,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f>SUMIF(E$2:E$5,$P14,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1091,27 +1091,27 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2">
-        <f>SUM(S15:W15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S15" s="2">
-        <f>SUMIF(A$2:A$5,$P15,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <f>SUMIF(B$2:B$5,$P15,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <f>SUMIF(C$2:C$5,$P15,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <f>SUMIF(D$2:D$5,$P15,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V15" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W15">
-        <f>SUMIF(E$2:E$5,$P15,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1131,27 +1131,27 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2">
-        <f>SUM(S16:W16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S16" s="2">
-        <f>SUMIF(A$2:A$5,$P16,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <f>SUMIF(B$2:B$5,$P16,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <f>SUMIF(C$2:C$5,$P16,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <f>SUMIF(D$2:D$5,$P16,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W16">
-        <f>SUMIF(E$2:E$5,$P16,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1171,27 +1171,27 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2">
-        <f>SUM(S17:W17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S17" s="2">
-        <f>SUMIF(A$2:A$5,$P17,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <f>SUMIF(B$2:B$5,$P17,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <f>SUMIF(C$2:C$5,$P17,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <f>SUMIF(D$2:D$5,$P17,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W17">
-        <f>SUMIF(E$2:E$5,$P17,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1211,27 +1211,27 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2">
-        <f>SUM(S18:W18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S18" s="2">
-        <f>SUMIF(A$2:A$5,$P18,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <f>SUMIF(B$2:B$5,$P18,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <f>SUMIF(C$2:C$5,$P18,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <f>SUMIF(D$2:D$5,$P18,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" ref="T18:T20" si="4">SUMIF(B:B,$P18,$J:$J )</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="2">
+        <f t="shared" ref="U18:U20" si="5">SUMIF(C:C,$P18,$J:$J )</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="2">
+        <f t="shared" ref="V18:V20" si="6">SUMIF(D:D,$P18,$J:$J )</f>
         <v>0</v>
       </c>
       <c r="W18">
-        <f>SUMIF(E$2:E$5,$P18,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1251,27 +1251,27 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2">
-        <f>SUM(S19:W19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S19" s="2">
-        <f>SUMIF(A$2:A$5,$P19,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <f>SUMIF(B$2:B$5,$P19,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <f>SUMIF(C$2:C$5,$P19,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <f>SUMIF(D$2:D$5,$P19,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="2">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W19">
-        <f>SUMIF(E$2:E$5,$P19,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1291,27 +1291,27 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2">
-        <f>SUM(S20:W20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S20" s="2">
-        <f>SUMIF(A$2:A$5,$P20,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <f>SUMIF(B$2:B$5,$P20,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <f>SUMIF(C$2:C$5,$P20,$J$2:$J$5)</f>
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <f>SUMIF(D$2:D$5,$P20,$J$2:$J$5)</f>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="2">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W20">
-        <f>SUMIF(E$2:E$5,$P20,$J$2:$J$5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1348,6 +1348,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
+      <c r="S22" s="2"/>
     </row>
     <row r="23" spans="3:23">
       <c r="C23" s="2"/>
@@ -2340,7 +2341,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <ignoredErrors>
-    <ignoredError sqref="S2:W20" emptyCellReference="1"/>
+    <ignoredError sqref="W20 W2 W3:W19 S2:V20" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>